<commit_message>
Cleaned up an issue in protective asset allocation and added a python for finance notebook.
</commit_message>
<xml_diff>
--- a/r/PAA.xlsx
+++ b/r/PAA.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17668"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\github\quant-intro\r\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sector portfolio" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>SPY</t>
   </si>
@@ -125,11 +130,17 @@
   <si>
     <t>Returns</t>
   </si>
+  <si>
+    <t>Number of assets</t>
+  </si>
+  <si>
+    <t>Lookback</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
@@ -222,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -259,6 +270,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,6 +289,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -317,7 +340,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,9 +373,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,6 +425,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2915,10 +2972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB253"/>
+  <dimension ref="A1:AC273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L238" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W259" sqref="W259"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N88" sqref="N88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6498,7 +6555,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="49" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>19</v>
       </c>
@@ -6576,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>20</v>
       </c>
@@ -6654,7 +6711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>21</v>
       </c>
@@ -6732,7 +6789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>22</v>
       </c>
@@ -6810,7 +6867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>23</v>
       </c>
@@ -6888,7 +6945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>24</v>
       </c>
@@ -6966,7 +7023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>25</v>
       </c>
@@ -7044,7 +7101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>26</v>
       </c>
@@ -7122,7 +7179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O57" s="1">
         <v>731</v>
       </c>
@@ -7167,7 +7224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O58" s="1">
         <v>732</v>
       </c>
@@ -7212,7 +7269,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>36</v>
+      </c>
       <c r="O59" s="1">
         <v>733</v>
       </c>
@@ -7257,7 +7317,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="60" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="15">
+        <v>0.54679999999999995</v>
+      </c>
+      <c r="D60" s="15">
+        <v>0.55120000000000002</v>
+      </c>
+      <c r="E60" s="15">
+        <v>0.57279999999999998</v>
+      </c>
+      <c r="F60" s="15">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="G60" s="15">
+        <v>0.56610000000000005</v>
+      </c>
+      <c r="H60" s="15">
+        <v>0.58440000000000003</v>
+      </c>
+      <c r="I60" s="15">
+        <v>0.57609999999999995</v>
+      </c>
+      <c r="J60" s="15">
+        <v>0.57520000000000004</v>
+      </c>
+      <c r="K60" s="15">
+        <v>0.57530000000000003</v>
+      </c>
+      <c r="L60" s="15">
+        <v>0.57650000000000001</v>
+      </c>
       <c r="O60" s="1">
         <v>734</v>
       </c>
@@ -7302,7 +7398,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="61" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.74539999999999995</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1.9743999999999999</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2.8694000000000002</v>
+      </c>
+      <c r="F61" s="2">
+        <v>3.5543</v>
+      </c>
+      <c r="G61" s="2">
+        <v>4.1184000000000003</v>
+      </c>
+      <c r="H61" s="2">
+        <v>4.5819999999999999</v>
+      </c>
+      <c r="I61" s="2">
+        <v>4.9973999999999998</v>
+      </c>
+      <c r="J61" s="2">
+        <v>5.4039999999999999</v>
+      </c>
+      <c r="K61" s="2">
+        <v>5.7881</v>
+      </c>
+      <c r="L61" s="2">
+        <v>6.2361000000000004</v>
+      </c>
       <c r="O61" s="1">
         <v>735</v>
       </c>
@@ -7347,7 +7476,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="62" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>3</v>
+      </c>
+      <c r="C62" s="15">
+        <v>0.46210000000000001</v>
+      </c>
+      <c r="D62" s="15">
+        <v>1.4185000000000001</v>
+      </c>
+      <c r="E62" s="15">
+        <v>2.2021000000000002</v>
+      </c>
+      <c r="F62" s="15">
+        <v>2.8776000000000002</v>
+      </c>
+      <c r="G62" s="15">
+        <v>3.3572000000000002</v>
+      </c>
+      <c r="H62" s="15">
+        <v>3.7871999999999999</v>
+      </c>
+      <c r="I62" s="15">
+        <v>4.1780999999999997</v>
+      </c>
+      <c r="J62" s="15">
+        <v>4.5503999999999998</v>
+      </c>
+      <c r="K62" s="15">
+        <v>4.9122000000000003</v>
+      </c>
+      <c r="L62" s="15">
+        <v>5.3582999999999998</v>
+      </c>
       <c r="O62" s="1">
         <v>736</v>
       </c>
@@ -7392,7 +7554,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="63" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.374</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1.4333</v>
+      </c>
+      <c r="E63" s="2">
+        <v>2.1886000000000001</v>
+      </c>
+      <c r="F63" s="2">
+        <v>2.7574000000000001</v>
+      </c>
+      <c r="G63" s="2">
+        <v>3.2480000000000002</v>
+      </c>
+      <c r="H63" s="2">
+        <v>3.6711999999999998</v>
+      </c>
+      <c r="I63" s="2">
+        <v>4.1120999999999999</v>
+      </c>
+      <c r="J63" s="2">
+        <v>4.4695</v>
+      </c>
+      <c r="K63" s="2">
+        <v>4.8483000000000001</v>
+      </c>
+      <c r="L63" s="2">
+        <v>5.3586999999999998</v>
+      </c>
       <c r="O63" s="1">
         <v>737</v>
       </c>
@@ -7437,7 +7632,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="64" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
+        <v>5</v>
+      </c>
+      <c r="C64" s="15">
+        <v>0.3029</v>
+      </c>
+      <c r="D64" s="15">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="E64" s="15">
+        <v>1.8982000000000001</v>
+      </c>
+      <c r="F64" s="15">
+        <v>2.4567000000000001</v>
+      </c>
+      <c r="G64" s="15">
+        <v>2.8864999999999998</v>
+      </c>
+      <c r="H64" s="15">
+        <v>3.3329</v>
+      </c>
+      <c r="I64" s="15">
+        <v>3.7313999999999998</v>
+      </c>
+      <c r="J64" s="15">
+        <v>4.1044</v>
+      </c>
+      <c r="K64" s="15">
+        <v>4.5145</v>
+      </c>
+      <c r="L64" s="15">
+        <v>5.0354999999999999</v>
+      </c>
       <c r="O64" s="1">
         <v>738</v>
       </c>
@@ -7482,7 +7710,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="65" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>6</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.22450000000000001</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1.1016999999999999</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1.7474000000000001</v>
+      </c>
+      <c r="F65" s="2">
+        <v>2.254</v>
+      </c>
+      <c r="G65" s="2">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="H65" s="2">
+        <v>3.0192000000000001</v>
+      </c>
+      <c r="I65" s="2">
+        <v>3.3919999999999999</v>
+      </c>
+      <c r="J65" s="2">
+        <v>3.6909999999999998</v>
+      </c>
+      <c r="K65" s="2">
+        <v>4.0608000000000004</v>
+      </c>
+      <c r="L65" s="2">
+        <v>4.5631000000000004</v>
+      </c>
       <c r="O65" s="1">
         <v>739</v>
       </c>
@@ -7527,7 +7788,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="66" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>7</v>
+      </c>
+      <c r="C66" s="15">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="D66" s="15">
+        <v>1.0561</v>
+      </c>
+      <c r="E66" s="15">
+        <v>1.7546999999999999</v>
+      </c>
+      <c r="F66" s="15">
+        <v>2.2168999999999999</v>
+      </c>
+      <c r="G66" s="15">
+        <v>2.5966999999999998</v>
+      </c>
+      <c r="H66" s="15">
+        <v>2.8965999999999998</v>
+      </c>
+      <c r="I66" s="15">
+        <v>3.2170999999999998</v>
+      </c>
+      <c r="J66" s="15">
+        <v>3.5714000000000001</v>
+      </c>
+      <c r="K66" s="15">
+        <v>3.9007000000000001</v>
+      </c>
+      <c r="L66" s="15">
+        <v>4.3829000000000002</v>
+      </c>
       <c r="O66" s="1">
         <v>740</v>
       </c>
@@ -7572,7 +7866,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="67" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>8</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.2717</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1.1102000000000001</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1.7212000000000001</v>
+      </c>
+      <c r="F67" s="2">
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="G67" s="2">
+        <v>2.5394999999999999</v>
+      </c>
+      <c r="H67" s="2">
+        <v>2.847</v>
+      </c>
+      <c r="I67" s="2">
+        <v>3.1486999999999998</v>
+      </c>
+      <c r="J67" s="2">
+        <v>3.4422000000000001</v>
+      </c>
+      <c r="K67" s="2">
+        <v>3.8208000000000002</v>
+      </c>
+      <c r="L67" s="2">
+        <v>4.2415000000000003</v>
+      </c>
       <c r="O67" s="1">
         <v>741</v>
       </c>
@@ -7617,7 +7944,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="68" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>9</v>
+      </c>
+      <c r="C68" s="15">
+        <v>0.249</v>
+      </c>
+      <c r="D68" s="15">
+        <v>0.99519999999999997</v>
+      </c>
+      <c r="E68" s="15">
+        <v>1.6627000000000001</v>
+      </c>
+      <c r="F68" s="15">
+        <v>2.0406</v>
+      </c>
+      <c r="G68" s="15">
+        <v>2.4184999999999999</v>
+      </c>
+      <c r="H68" s="15">
+        <v>2.6884000000000001</v>
+      </c>
+      <c r="I68" s="15">
+        <v>3.0369000000000002</v>
+      </c>
+      <c r="J68" s="15">
+        <v>3.3308</v>
+      </c>
+      <c r="K68" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="L68" s="15">
+        <v>4.0751999999999997</v>
+      </c>
       <c r="O68" s="1">
         <v>742</v>
       </c>
@@ -7662,7 +8022,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="69" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
+        <v>10</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.25619999999999998</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1.0631999999999999</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1.5689</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1.9493</v>
+      </c>
+      <c r="G69" s="2">
+        <v>2.2970000000000002</v>
+      </c>
+      <c r="H69" s="2">
+        <v>2.5857999999999999</v>
+      </c>
+      <c r="I69" s="2">
+        <v>2.9628999999999999</v>
+      </c>
+      <c r="J69" s="2">
+        <v>3.2124000000000001</v>
+      </c>
+      <c r="K69" s="2">
+        <v>3.5301</v>
+      </c>
+      <c r="L69" s="2">
+        <v>3.9043999999999999</v>
+      </c>
       <c r="O69" s="1">
         <v>743</v>
       </c>
@@ -7707,7 +8100,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="70" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="1">
+        <v>11</v>
+      </c>
+      <c r="C70" s="15">
+        <v>0.12130000000000001</v>
+      </c>
+      <c r="D70" s="15">
+        <v>0.97840000000000005</v>
+      </c>
+      <c r="E70" s="15">
+        <v>1.5111000000000001</v>
+      </c>
+      <c r="F70" s="15">
+        <v>1.8421000000000001</v>
+      </c>
+      <c r="G70" s="15">
+        <v>2.2021000000000002</v>
+      </c>
+      <c r="H70" s="15">
+        <v>2.5045000000000002</v>
+      </c>
+      <c r="I70" s="15">
+        <v>2.7917000000000001</v>
+      </c>
+      <c r="J70" s="15">
+        <v>3.0594000000000001</v>
+      </c>
+      <c r="K70" s="15">
+        <v>3.3763999999999998</v>
+      </c>
+      <c r="L70" s="15">
+        <v>3.7338</v>
+      </c>
       <c r="O70" s="1">
         <v>744</v>
       </c>
@@ -7752,7 +8178,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="71" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="1">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1.4819</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1.8220000000000001</v>
+      </c>
+      <c r="G71" s="2">
+        <v>2.1941999999999999</v>
+      </c>
+      <c r="H71" s="2">
+        <v>2.4697</v>
+      </c>
+      <c r="I71" s="2">
+        <v>2.7597999999999998</v>
+      </c>
+      <c r="J71" s="2">
+        <v>2.9952999999999999</v>
+      </c>
+      <c r="K71" s="2">
+        <v>3.3138999999999998</v>
+      </c>
+      <c r="L71" s="2">
+        <v>3.6528999999999998</v>
+      </c>
       <c r="O71" s="1">
         <v>745</v>
       </c>
@@ -7797,7 +8256,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="72" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="1">
+        <v>13</v>
+      </c>
+      <c r="C72" s="15">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="D72" s="15">
+        <v>0.9133</v>
+      </c>
+      <c r="E72" s="15">
+        <v>1.3701000000000001</v>
+      </c>
+      <c r="F72" s="15">
+        <v>1.7945</v>
+      </c>
+      <c r="G72" s="15">
+        <v>2.1147999999999998</v>
+      </c>
+      <c r="H72" s="15">
+        <v>2.4039999999999999</v>
+      </c>
+      <c r="I72" s="15">
+        <v>2.6528</v>
+      </c>
+      <c r="J72" s="15">
+        <v>2.9117999999999999</v>
+      </c>
+      <c r="K72" s="15">
+        <v>3.2273000000000001</v>
+      </c>
+      <c r="L72" s="15">
+        <v>3.5543999999999998</v>
+      </c>
       <c r="O72" s="1">
         <v>746</v>
       </c>
@@ -7842,7 +8334,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="73" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="1">
+        <v>14</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.91969999999999996</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1.3581000000000001</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1.746</v>
+      </c>
+      <c r="G73" s="2">
+        <v>2.0287999999999999</v>
+      </c>
+      <c r="H73" s="2">
+        <v>2.3066</v>
+      </c>
+      <c r="I73" s="2">
+        <v>2.5773000000000001</v>
+      </c>
+      <c r="J73" s="2">
+        <v>2.8683000000000001</v>
+      </c>
+      <c r="K73" s="2">
+        <v>3.1467000000000001</v>
+      </c>
+      <c r="L73" s="2">
+        <v>3.4859</v>
+      </c>
       <c r="O73" s="1">
         <v>747</v>
       </c>
@@ -7887,7 +8412,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="74" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="1">
+        <v>15</v>
+      </c>
+      <c r="C74" s="15">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="D74" s="15">
+        <v>0.94369999999999998</v>
+      </c>
+      <c r="E74" s="15">
+        <v>1.3178000000000001</v>
+      </c>
+      <c r="F74" s="15">
+        <v>1.6931</v>
+      </c>
+      <c r="G74" s="15">
+        <v>1.9577</v>
+      </c>
+      <c r="H74" s="15">
+        <v>2.2789999999999999</v>
+      </c>
+      <c r="I74" s="15">
+        <v>2.5205000000000002</v>
+      </c>
+      <c r="J74" s="15">
+        <v>2.8128000000000002</v>
+      </c>
+      <c r="K74" s="15">
+        <v>3.0670000000000002</v>
+      </c>
+      <c r="L74" s="15">
+        <v>3.3933</v>
+      </c>
       <c r="O74" s="1">
         <v>748</v>
       </c>
@@ -7932,7 +8490,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="75" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="1">
+        <v>16</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.36130000000000001</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.85140000000000005</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1.7016</v>
+      </c>
+      <c r="G75" s="2">
+        <v>1.9285000000000001</v>
+      </c>
+      <c r="H75" s="2">
+        <v>2.2471000000000001</v>
+      </c>
+      <c r="I75" s="2">
+        <v>2.4992999999999999</v>
+      </c>
+      <c r="J75" s="2">
+        <v>2.7408999999999999</v>
+      </c>
+      <c r="K75" s="2">
+        <v>2.9901</v>
+      </c>
+      <c r="L75" s="2">
+        <v>3.3006000000000002</v>
+      </c>
       <c r="O75" s="1">
         <v>749</v>
       </c>
@@ -7977,7 +8568,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="76" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="1">
+        <v>17</v>
+      </c>
+      <c r="C76" s="15">
+        <v>0.33379999999999999</v>
+      </c>
+      <c r="D76" s="15">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="E76" s="15">
+        <v>1.3048</v>
+      </c>
+      <c r="F76" s="15">
+        <v>1.6529</v>
+      </c>
+      <c r="G76" s="15">
+        <v>1.9287000000000001</v>
+      </c>
+      <c r="H76" s="15">
+        <v>2.1855000000000002</v>
+      </c>
+      <c r="I76" s="15">
+        <v>2.4188999999999998</v>
+      </c>
+      <c r="J76" s="15">
+        <v>2.6551</v>
+      </c>
+      <c r="K76" s="15">
+        <v>2.9119999999999999</v>
+      </c>
+      <c r="L76" s="15">
+        <v>3.2054999999999998</v>
+      </c>
       <c r="O76" s="1">
         <v>750</v>
       </c>
@@ -8022,7 +8646,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="77" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="1">
+        <v>18</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.27229999999999999</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1.2786999999999999</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1.5924</v>
+      </c>
+      <c r="G77" s="2">
+        <v>1.8442000000000001</v>
+      </c>
+      <c r="H77" s="2">
+        <v>2.0994999999999999</v>
+      </c>
+      <c r="I77" s="2">
+        <v>2.3403</v>
+      </c>
+      <c r="J77" s="2">
+        <v>2.5720000000000001</v>
+      </c>
+      <c r="K77" s="2">
+        <v>2.8464999999999998</v>
+      </c>
+      <c r="L77" s="2">
+        <v>3.1236999999999999</v>
+      </c>
       <c r="O77" s="1">
         <v>751</v>
       </c>
@@ -8067,7 +8724,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="78" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="1">
+        <v>19</v>
+      </c>
+      <c r="C78" s="15">
+        <v>0.3201</v>
+      </c>
+      <c r="D78" s="15">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="E78" s="15">
+        <v>1.3126</v>
+      </c>
+      <c r="F78" s="15">
+        <v>1.5827</v>
+      </c>
+      <c r="G78" s="15">
+        <v>1.8310999999999999</v>
+      </c>
+      <c r="H78" s="15">
+        <v>2.0905999999999998</v>
+      </c>
+      <c r="I78" s="15">
+        <v>2.3523999999999998</v>
+      </c>
+      <c r="J78" s="15">
+        <v>2.5855999999999999</v>
+      </c>
+      <c r="K78" s="15">
+        <v>2.8586999999999998</v>
+      </c>
+      <c r="L78" s="15">
+        <v>3.1322000000000001</v>
+      </c>
       <c r="O78" s="1">
         <v>752</v>
       </c>
@@ -8112,7 +8802,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="79" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="1">
+        <v>20</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.85619999999999996</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1.3018000000000001</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1.5944</v>
+      </c>
+      <c r="G79" s="2">
+        <v>1.8117000000000001</v>
+      </c>
+      <c r="H79" s="2">
+        <v>2.0457000000000001</v>
+      </c>
+      <c r="I79" s="2">
+        <v>2.3172000000000001</v>
+      </c>
+      <c r="J79" s="2">
+        <v>2.5402</v>
+      </c>
+      <c r="K79" s="2">
+        <v>2.8052000000000001</v>
+      </c>
+      <c r="L79" s="2">
+        <v>3.0712000000000002</v>
+      </c>
       <c r="O79" s="1">
         <v>753</v>
       </c>
@@ -8157,7 +8880,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="80" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="1">
+        <v>21</v>
+      </c>
+      <c r="C80" s="15">
+        <v>0.35970000000000002</v>
+      </c>
+      <c r="D80" s="15">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="E80" s="15">
+        <v>1.2862</v>
+      </c>
+      <c r="F80" s="15">
+        <v>1.5346</v>
+      </c>
+      <c r="G80" s="15">
+        <v>1.7608999999999999</v>
+      </c>
+      <c r="H80" s="15">
+        <v>2.0023</v>
+      </c>
+      <c r="I80" s="15">
+        <v>2.2549999999999999</v>
+      </c>
+      <c r="J80" s="15">
+        <v>2.4889000000000001</v>
+      </c>
+      <c r="K80" s="15">
+        <v>2.7549999999999999</v>
+      </c>
+      <c r="L80" s="15">
+        <v>3.0301999999999998</v>
+      </c>
       <c r="O80" s="1">
         <v>754</v>
       </c>
@@ -8202,7 +8958,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="81" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="1">
+        <v>22</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.79010000000000002</v>
+      </c>
+      <c r="E81" s="2">
+        <v>1.2438</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1.5278</v>
+      </c>
+      <c r="G81" s="2">
+        <v>1.7381</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1.9691000000000001</v>
+      </c>
+      <c r="I81" s="2">
+        <v>2.2370999999999999</v>
+      </c>
+      <c r="J81" s="2">
+        <v>2.4531999999999998</v>
+      </c>
+      <c r="K81" s="2">
+        <v>2.7185000000000001</v>
+      </c>
+      <c r="L81" s="2">
+        <v>2.988</v>
+      </c>
       <c r="O81" s="1">
         <v>755</v>
       </c>
@@ -8247,7 +9036,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="82" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="1">
+        <v>23</v>
+      </c>
+      <c r="C82" s="15">
+        <v>0.37080000000000002</v>
+      </c>
+      <c r="D82" s="15">
+        <v>0.87829999999999997</v>
+      </c>
+      <c r="E82" s="15">
+        <v>1.2101999999999999</v>
+      </c>
+      <c r="F82" s="15">
+        <v>1.5530999999999999</v>
+      </c>
+      <c r="G82" s="15">
+        <v>1.7124999999999999</v>
+      </c>
+      <c r="H82" s="15">
+        <v>1.9292</v>
+      </c>
+      <c r="I82" s="15">
+        <v>2.2120000000000002</v>
+      </c>
+      <c r="J82" s="15">
+        <v>2.4232</v>
+      </c>
+      <c r="K82" s="15">
+        <v>2.6701999999999999</v>
+      </c>
+      <c r="L82" s="15">
+        <v>2.9323999999999999</v>
+      </c>
       <c r="O82" s="1">
         <v>756</v>
       </c>
@@ -8292,7 +9114,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="83" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
+        <v>24</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.87690000000000001</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1.2283999999999999</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1.5674999999999999</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1.7716000000000001</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1.9577</v>
+      </c>
+      <c r="I83" s="2">
+        <v>2.2029000000000001</v>
+      </c>
+      <c r="J83" s="2">
+        <v>2.4171999999999998</v>
+      </c>
+      <c r="K83" s="2">
+        <v>2.6493000000000002</v>
+      </c>
+      <c r="L83" s="2">
+        <v>2.9241999999999999</v>
+      </c>
       <c r="O83" s="1">
         <v>757</v>
       </c>
@@ -8337,7 +9192,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="84" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
+        <v>25</v>
+      </c>
+      <c r="C84" s="15">
+        <v>0.33389999999999997</v>
+      </c>
+      <c r="D84" s="15">
+        <v>0.86739999999999995</v>
+      </c>
+      <c r="E84" s="15">
+        <v>1.2239</v>
+      </c>
+      <c r="F84" s="15">
+        <v>1.5407</v>
+      </c>
+      <c r="G84" s="15">
+        <v>1.7452000000000001</v>
+      </c>
+      <c r="H84" s="15">
+        <v>1.9316</v>
+      </c>
+      <c r="I84" s="15">
+        <v>2.1934</v>
+      </c>
+      <c r="J84" s="15">
+        <v>2.3723000000000001</v>
+      </c>
+      <c r="K84" s="15">
+        <v>2.6118999999999999</v>
+      </c>
+      <c r="L84" s="15">
+        <v>2.88</v>
+      </c>
       <c r="O84" s="1">
         <v>758</v>
       </c>
@@ -8382,7 +9270,40 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="85" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="1">
+        <v>26</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.35360000000000003</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1.2052</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1.5769</v>
+      </c>
+      <c r="G85" s="2">
+        <v>1.7129000000000001</v>
+      </c>
+      <c r="H85" s="2">
+        <v>1.9156</v>
+      </c>
+      <c r="I85" s="2">
+        <v>2.1808000000000001</v>
+      </c>
+      <c r="J85" s="2">
+        <v>2.3917999999999999</v>
+      </c>
+      <c r="K85" s="2">
+        <v>2.605</v>
+      </c>
+      <c r="L85" s="2">
+        <v>2.8601000000000001</v>
+      </c>
       <c r="O85" s="1">
         <v>759</v>
       </c>
@@ -8427,7 +9348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O86" s="1">
         <v>760</v>
       </c>
@@ -8472,7 +9393,10 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="87" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>36</v>
+      </c>
       <c r="O87" s="1">
         <v>761</v>
       </c>
@@ -8517,7 +9441,46 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="88" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" s="15">
+        <v>-7.1900000000000006E-2</v>
+      </c>
+      <c r="D88" s="15">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.47470000000000001</v>
+      </c>
+      <c r="F88" s="15">
+        <v>0.74209999999999998</v>
+      </c>
+      <c r="G88" s="15">
+        <v>1.0041</v>
+      </c>
+      <c r="H88" s="15">
+        <v>1.1628000000000001</v>
+      </c>
+      <c r="I88" s="15">
+        <v>1.3179000000000001</v>
+      </c>
+      <c r="J88" s="15">
+        <v>1.4596</v>
+      </c>
+      <c r="K88" s="15">
+        <v>1.6156999999999999</v>
+      </c>
+      <c r="L88" s="15">
+        <v>1.7465999999999999</v>
+      </c>
+      <c r="M88" s="15">
+        <v>1.9234</v>
+      </c>
       <c r="O88" s="1">
         <v>762</v>
       </c>
@@ -8562,7 +9525,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="89" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="1">
+        <v>2</v>
+      </c>
+      <c r="C89" s="2">
+        <v>-0.2046</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.1336</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="F89" s="2">
+        <v>0.75719999999999998</v>
+      </c>
+      <c r="G89" s="2">
+        <v>0.94430000000000003</v>
+      </c>
+      <c r="H89" s="2">
+        <v>1.1251</v>
+      </c>
+      <c r="I89" s="2">
+        <v>1.2995000000000001</v>
+      </c>
+      <c r="J89" s="2">
+        <v>1.4377</v>
+      </c>
+      <c r="K89" s="2">
+        <v>1.5696000000000001</v>
+      </c>
+      <c r="L89" s="2">
+        <v>1.7089000000000001</v>
+      </c>
+      <c r="M89" s="2">
+        <v>1.8847</v>
+      </c>
       <c r="O89" s="1">
         <v>763</v>
       </c>
@@ -8607,7 +9606,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="90" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="1">
+        <v>3</v>
+      </c>
+      <c r="C90" s="15">
+        <v>-0.1474</v>
+      </c>
+      <c r="D90" s="15">
+        <v>0.2321</v>
+      </c>
+      <c r="E90" s="15">
+        <v>0.4773</v>
+      </c>
+      <c r="F90" s="15">
+        <v>0.75719999999999998</v>
+      </c>
+      <c r="G90" s="15">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="H90" s="15">
+        <v>1.1152</v>
+      </c>
+      <c r="I90" s="15">
+        <v>1.3006</v>
+      </c>
+      <c r="J90" s="15">
+        <v>1.4523999999999999</v>
+      </c>
+      <c r="K90" s="15">
+        <v>1.5755999999999999</v>
+      </c>
+      <c r="L90" s="15">
+        <v>1.6981999999999999</v>
+      </c>
+      <c r="M90" s="15">
+        <v>1.8743000000000001</v>
+      </c>
       <c r="O90" s="1">
         <v>764</v>
       </c>
@@ -8652,7 +9687,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="91" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="1">
+        <v>4</v>
+      </c>
+      <c r="C91" s="2">
+        <v>-0.1179</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="E91" s="2">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="F91" s="2">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="G91" s="2">
+        <v>0.94330000000000003</v>
+      </c>
+      <c r="H91" s="2">
+        <v>1.1394</v>
+      </c>
+      <c r="I91" s="2">
+        <v>1.2966</v>
+      </c>
+      <c r="J91" s="2">
+        <v>1.4418</v>
+      </c>
+      <c r="K91" s="2">
+        <v>1.5704</v>
+      </c>
+      <c r="L91" s="2">
+        <v>1.6809000000000001</v>
+      </c>
+      <c r="M91" s="2">
+        <v>1.853</v>
+      </c>
       <c r="O91" s="1">
         <v>765</v>
       </c>
@@ -8697,7 +9768,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="92" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="1">
+        <v>5</v>
+      </c>
+      <c r="C92" s="15">
+        <v>-6.9500000000000006E-2</v>
+      </c>
+      <c r="D92" s="15">
+        <v>0.1547</v>
+      </c>
+      <c r="E92" s="15">
+        <v>0.52290000000000003</v>
+      </c>
+      <c r="F92" s="15">
+        <v>0.8286</v>
+      </c>
+      <c r="G92" s="15">
+        <v>0.9778</v>
+      </c>
+      <c r="H92" s="15">
+        <v>1.1621999999999999</v>
+      </c>
+      <c r="I92" s="15">
+        <v>1.3121</v>
+      </c>
+      <c r="J92" s="15">
+        <v>1.4473</v>
+      </c>
+      <c r="K92" s="15">
+        <v>1.5812999999999999</v>
+      </c>
+      <c r="L92" s="15">
+        <v>1.7063999999999999</v>
+      </c>
+      <c r="M92" s="15">
+        <v>1.8568</v>
+      </c>
       <c r="O92" s="1">
         <v>766</v>
       </c>
@@ -8742,7 +9849,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="93" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="1">
+        <v>6</v>
+      </c>
+      <c r="C93" s="2">
+        <v>-5.6099999999999997E-2</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.1759</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0.51180000000000003</v>
+      </c>
+      <c r="F93" s="2">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="G93" s="2">
+        <v>0.98470000000000002</v>
+      </c>
+      <c r="H93" s="2">
+        <v>1.1478999999999999</v>
+      </c>
+      <c r="I93" s="2">
+        <v>1.2734000000000001</v>
+      </c>
+      <c r="J93" s="2">
+        <v>1.4018999999999999</v>
+      </c>
+      <c r="K93" s="2">
+        <v>1.5356000000000001</v>
+      </c>
+      <c r="L93" s="2">
+        <v>1.6548</v>
+      </c>
+      <c r="M93" s="2">
+        <v>1.8204</v>
+      </c>
       <c r="O93" s="1">
         <v>767</v>
       </c>
@@ -8787,7 +9930,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="1">
+        <v>7</v>
+      </c>
+      <c r="C94" s="15">
+        <v>-0.1046</v>
+      </c>
+      <c r="D94" s="15">
+        <v>0.15939999999999999</v>
+      </c>
+      <c r="E94" s="15">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="F94" s="15">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="G94" s="15">
+        <v>0.96509999999999996</v>
+      </c>
+      <c r="H94" s="15">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="I94" s="15">
+        <v>1.2253000000000001</v>
+      </c>
+      <c r="J94" s="15">
+        <v>1.3678999999999999</v>
+      </c>
+      <c r="K94" s="15">
+        <v>1.5027999999999999</v>
+      </c>
+      <c r="L94" s="15">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="M94" s="15">
+        <v>1.7836000000000001</v>
+      </c>
       <c r="O94" s="1">
         <v>768</v>
       </c>
@@ -8832,7 +10011,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="1">
+        <v>8</v>
+      </c>
+      <c r="C95" s="2">
+        <v>-3.9600000000000003E-2</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0.18690000000000001</v>
+      </c>
+      <c r="E95" s="2">
+        <v>0.59279999999999999</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="G95" s="2">
+        <v>1.0001</v>
+      </c>
+      <c r="H95" s="2">
+        <v>1.1462000000000001</v>
+      </c>
+      <c r="I95" s="2">
+        <v>1.2425999999999999</v>
+      </c>
+      <c r="J95" s="2">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="K95" s="2">
+        <v>1.5331999999999999</v>
+      </c>
+      <c r="L95" s="2">
+        <v>1.6366000000000001</v>
+      </c>
+      <c r="M95" s="2">
+        <v>1.7931999999999999</v>
+      </c>
       <c r="O95" s="1">
         <v>769</v>
       </c>
@@ -8877,7 +10092,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="96" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="1">
+        <v>9</v>
+      </c>
+      <c r="C96" s="15">
+        <v>-6.4699999999999994E-2</v>
+      </c>
+      <c r="D96" s="15">
+        <v>0.22819999999999999</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0.58430000000000004</v>
+      </c>
+      <c r="F96" s="15">
+        <v>0.8125</v>
+      </c>
+      <c r="G96" s="15">
+        <v>1.0165999999999999</v>
+      </c>
+      <c r="H96" s="15">
+        <v>1.1334</v>
+      </c>
+      <c r="I96" s="15">
+        <v>1.2347999999999999</v>
+      </c>
+      <c r="J96" s="15">
+        <v>1.3905000000000001</v>
+      </c>
+      <c r="K96" s="15">
+        <v>1.5277000000000001</v>
+      </c>
+      <c r="L96" s="15">
+        <v>1.6316999999999999</v>
+      </c>
+      <c r="M96" s="15">
+        <v>1.7903</v>
+      </c>
       <c r="O96" s="1">
         <v>770</v>
       </c>
@@ -8922,7 +10173,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="97" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="1">
+        <v>10</v>
+      </c>
+      <c r="C97" s="2">
+        <v>-3.0800000000000001E-2</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.2681</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0.59889999999999999</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1.1384000000000001</v>
+      </c>
+      <c r="I97" s="2">
+        <v>1.2388999999999999</v>
+      </c>
+      <c r="J97" s="2">
+        <v>1.3727</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1.5173000000000001</v>
+      </c>
+      <c r="L97" s="2">
+        <v>1.6087</v>
+      </c>
+      <c r="M97" s="2">
+        <v>1.7613000000000001</v>
+      </c>
       <c r="O97" s="1">
         <v>771</v>
       </c>
@@ -8967,7 +10254,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="98" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="1">
+        <v>11</v>
+      </c>
+      <c r="C98" s="15">
+        <v>1.06E-2</v>
+      </c>
+      <c r="D98" s="15">
+        <v>0.29249999999999998</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0.63119999999999998</v>
+      </c>
+      <c r="F98" s="15">
+        <v>0.76859999999999995</v>
+      </c>
+      <c r="G98" s="15">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="H98" s="15">
+        <v>1.0817000000000001</v>
+      </c>
+      <c r="I98" s="15">
+        <v>1.1938</v>
+      </c>
+      <c r="J98" s="15">
+        <v>1.3302</v>
+      </c>
+      <c r="K98" s="15">
+        <v>1.4573</v>
+      </c>
+      <c r="L98" s="15">
+        <v>1.5418000000000001</v>
+      </c>
+      <c r="M98" s="15">
+        <v>1.7085999999999999</v>
+      </c>
       <c r="O98" s="1">
         <v>772</v>
       </c>
@@ -9012,7 +10335,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="1">
+        <v>12</v>
+      </c>
+      <c r="C99" s="2">
+        <v>-1.47E-2</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.25119999999999998</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.73619999999999997</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0.92349999999999999</v>
+      </c>
+      <c r="H99" s="2">
+        <v>1.0064</v>
+      </c>
+      <c r="I99" s="2">
+        <v>1.1492</v>
+      </c>
+      <c r="J99" s="2">
+        <v>1.2811999999999999</v>
+      </c>
+      <c r="K99" s="2">
+        <v>1.4052</v>
+      </c>
+      <c r="L99" s="2">
+        <v>1.4846999999999999</v>
+      </c>
+      <c r="M99" s="2">
+        <v>1.6549</v>
+      </c>
       <c r="O99" s="1">
         <v>773</v>
       </c>
@@ -9057,7 +10416,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="100" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
+        <v>13</v>
+      </c>
+      <c r="C100" s="15">
+        <v>-6.2300000000000001E-2</v>
+      </c>
+      <c r="D100" s="15">
+        <v>0.2394</v>
+      </c>
+      <c r="E100" s="15">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="F100" s="15">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="G100" s="15">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="H100" s="15">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="I100" s="15">
+        <v>1.1122000000000001</v>
+      </c>
+      <c r="J100" s="15">
+        <v>1.2435</v>
+      </c>
+      <c r="K100" s="15">
+        <v>1.3653</v>
+      </c>
+      <c r="L100" s="15">
+        <v>1.4584999999999999</v>
+      </c>
+      <c r="M100" s="15">
+        <v>1.613</v>
+      </c>
       <c r="O100" s="1">
         <v>774</v>
       </c>
@@ -9102,7 +10497,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="101" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="1">
+        <v>14</v>
+      </c>
+      <c r="C101" s="2">
+        <v>-3.1600000000000003E-2</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.20810000000000001</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0.5726</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.69869999999999999</v>
+      </c>
+      <c r="G101" s="2">
+        <v>0.86909999999999998</v>
+      </c>
+      <c r="H101" s="2">
+        <v>0.97540000000000004</v>
+      </c>
+      <c r="I101" s="2">
+        <v>1.1108</v>
+      </c>
+      <c r="J101" s="2">
+        <v>1.2426999999999999</v>
+      </c>
+      <c r="K101" s="2">
+        <v>1.3499000000000001</v>
+      </c>
+      <c r="L101" s="2">
+        <v>1.4494</v>
+      </c>
+      <c r="M101" s="2">
+        <v>1.5940000000000001</v>
+      </c>
       <c r="O101" s="1">
         <v>775</v>
       </c>
@@ -9147,7 +10578,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="102" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="1">
+        <v>15</v>
+      </c>
+      <c r="C102" s="15">
+        <v>-7.2800000000000004E-2</v>
+      </c>
+      <c r="D102" s="15">
+        <v>0.19359999999999999</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.54159999999999997</v>
+      </c>
+      <c r="F102" s="15">
+        <v>0.69259999999999999</v>
+      </c>
+      <c r="G102" s="15">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="H102" s="15">
+        <v>0.96330000000000005</v>
+      </c>
+      <c r="I102" s="15">
+        <v>1.0981000000000001</v>
+      </c>
+      <c r="J102" s="15">
+        <v>1.2232000000000001</v>
+      </c>
+      <c r="K102" s="15">
+        <v>1.3514999999999999</v>
+      </c>
+      <c r="L102" s="15">
+        <v>1.4501999999999999</v>
+      </c>
+      <c r="M102" s="15">
+        <v>1.5947</v>
+      </c>
       <c r="O102" s="1">
         <v>776</v>
       </c>
@@ -9192,7 +10659,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="103" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="1">
+        <v>16</v>
+      </c>
+      <c r="C103" s="2">
+        <v>-5.6399999999999999E-2</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0.58730000000000004</v>
+      </c>
+      <c r="F103" s="2">
+        <v>0.75819999999999999</v>
+      </c>
+      <c r="G103" s="2">
+        <v>0.91269999999999996</v>
+      </c>
+      <c r="H103" s="2">
+        <v>1.0194000000000001</v>
+      </c>
+      <c r="I103" s="2">
+        <v>1.1301000000000001</v>
+      </c>
+      <c r="J103" s="2">
+        <v>1.2838000000000001</v>
+      </c>
+      <c r="K103" s="2">
+        <v>1.4019999999999999</v>
+      </c>
+      <c r="L103" s="2">
+        <v>1.4899</v>
+      </c>
+      <c r="M103" s="2">
+        <v>1.6361000000000001</v>
+      </c>
       <c r="O103" s="1">
         <v>777</v>
       </c>
@@ -9237,7 +10740,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="104" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="1">
+        <v>17</v>
+      </c>
+      <c r="C104" s="15">
+        <v>-3.5999999999999997E-2</v>
+      </c>
+      <c r="D104" s="15">
+        <v>0.30349999999999999</v>
+      </c>
+      <c r="E104" s="15">
+        <v>0.58979999999999999</v>
+      </c>
+      <c r="F104" s="15">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="G104" s="15">
+        <v>0.89190000000000003</v>
+      </c>
+      <c r="H104" s="15">
+        <v>1.0033000000000001</v>
+      </c>
+      <c r="I104" s="15">
+        <v>1.1084000000000001</v>
+      </c>
+      <c r="J104" s="15">
+        <v>1.2517</v>
+      </c>
+      <c r="K104" s="15">
+        <v>1.3623000000000001</v>
+      </c>
+      <c r="L104" s="15">
+        <v>1.4599</v>
+      </c>
+      <c r="M104" s="15">
+        <v>1.5969</v>
+      </c>
       <c r="O104" s="1">
         <v>778</v>
       </c>
@@ -9282,7 +10821,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="105" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="1">
+        <v>18</v>
+      </c>
+      <c r="C105" s="2">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.31690000000000002</v>
+      </c>
+      <c r="E105" s="2">
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="F105" s="2">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="H105" s="2">
+        <v>1.0374000000000001</v>
+      </c>
+      <c r="I105" s="2">
+        <v>1.1283000000000001</v>
+      </c>
+      <c r="J105" s="2">
+        <v>1.2737000000000001</v>
+      </c>
+      <c r="K105" s="2">
+        <v>1.3873</v>
+      </c>
+      <c r="L105" s="2">
+        <v>1.4841</v>
+      </c>
+      <c r="M105" s="2">
+        <v>1.6071</v>
+      </c>
       <c r="O105" s="1">
         <v>779</v>
       </c>
@@ -9327,7 +10902,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="106" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="1">
+        <v>19</v>
+      </c>
+      <c r="C106" s="15">
+        <v>9.6699999999999994E-2</v>
+      </c>
+      <c r="D106" s="15">
+        <v>0.35880000000000001</v>
+      </c>
+      <c r="E106" s="15">
+        <v>0.59219999999999995</v>
+      </c>
+      <c r="F106" s="15">
+        <v>0.83150000000000002</v>
+      </c>
+      <c r="G106" s="15">
+        <v>0.95450000000000002</v>
+      </c>
+      <c r="H106" s="15">
+        <v>1.0768</v>
+      </c>
+      <c r="I106" s="15">
+        <v>1.1939</v>
+      </c>
+      <c r="J106" s="15">
+        <v>1.3139000000000001</v>
+      </c>
+      <c r="K106" s="15">
+        <v>1.4246000000000001</v>
+      </c>
+      <c r="L106" s="15">
+        <v>1.5204</v>
+      </c>
+      <c r="M106" s="15">
+        <v>1.6420999999999999</v>
+      </c>
       <c r="O106" s="1">
         <v>780</v>
       </c>
@@ -9372,7 +10983,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="107" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="1">
+        <v>20</v>
+      </c>
+      <c r="C107" s="2">
+        <v>0.14979999999999999</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0.44340000000000002</v>
+      </c>
+      <c r="E107" s="2">
+        <v>0.64929999999999999</v>
+      </c>
+      <c r="F107" s="2">
+        <v>0.88739999999999997</v>
+      </c>
+      <c r="G107" s="2">
+        <v>1.0448</v>
+      </c>
+      <c r="H107" s="2">
+        <v>1.1445000000000001</v>
+      </c>
+      <c r="I107" s="2">
+        <v>1.2529999999999999</v>
+      </c>
+      <c r="J107" s="2">
+        <v>1.355</v>
+      </c>
+      <c r="K107" s="2">
+        <v>1.4882</v>
+      </c>
+      <c r="L107" s="2">
+        <v>1.585</v>
+      </c>
+      <c r="M107" s="2">
+        <v>1.7113</v>
+      </c>
       <c r="O107" s="1">
         <v>781</v>
       </c>
@@ -9417,7 +11064,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="108" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="1">
+        <v>21</v>
+      </c>
+      <c r="C108" s="15">
+        <v>0.1762</v>
+      </c>
+      <c r="D108" s="15">
+        <v>0.47949999999999998</v>
+      </c>
+      <c r="E108" s="15">
+        <v>0.69889999999999997</v>
+      </c>
+      <c r="F108" s="15">
+        <v>0.89539999999999997</v>
+      </c>
+      <c r="G108" s="15">
+        <v>1.0497000000000001</v>
+      </c>
+      <c r="H108" s="15">
+        <v>1.1488</v>
+      </c>
+      <c r="I108" s="15">
+        <v>1.2515000000000001</v>
+      </c>
+      <c r="J108" s="15">
+        <v>1.3441000000000001</v>
+      </c>
+      <c r="K108" s="15">
+        <v>1.4837</v>
+      </c>
+      <c r="L108" s="15">
+        <v>1.5886</v>
+      </c>
+      <c r="M108" s="15">
+        <v>1.7071000000000001</v>
+      </c>
       <c r="O108" s="1">
         <v>782</v>
       </c>
@@ -9462,7 +11145,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="109" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="1">
+        <v>22</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.19670000000000001</v>
+      </c>
+      <c r="D109" s="2">
+        <v>0.49330000000000002</v>
+      </c>
+      <c r="E109" s="2">
+        <v>0.65369999999999995</v>
+      </c>
+      <c r="F109" s="2">
+        <v>0.86870000000000003</v>
+      </c>
+      <c r="G109" s="2">
+        <v>1.0450999999999999</v>
+      </c>
+      <c r="H109" s="2">
+        <v>1.1238999999999999</v>
+      </c>
+      <c r="I109" s="2">
+        <v>1.2153</v>
+      </c>
+      <c r="J109" s="2">
+        <v>1.3225</v>
+      </c>
+      <c r="K109" s="2">
+        <v>1.4869000000000001</v>
+      </c>
+      <c r="L109" s="2">
+        <v>1.5742</v>
+      </c>
+      <c r="M109" s="2">
+        <v>1.6922999999999999</v>
+      </c>
       <c r="O109" s="1">
         <v>783</v>
       </c>
@@ -9507,7 +11226,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="110" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="1">
+        <v>23</v>
+      </c>
+      <c r="C110" s="15">
+        <v>0.20019999999999999</v>
+      </c>
+      <c r="D110" s="15">
+        <v>0.4844</v>
+      </c>
+      <c r="E110" s="15">
+        <v>0.62929999999999997</v>
+      </c>
+      <c r="F110" s="15">
+        <v>0.85840000000000005</v>
+      </c>
+      <c r="G110" s="15">
+        <v>1.024</v>
+      </c>
+      <c r="H110" s="15">
+        <v>1.0894999999999999</v>
+      </c>
+      <c r="I110" s="15">
+        <v>1.1939</v>
+      </c>
+      <c r="J110" s="15">
+        <v>1.2963</v>
+      </c>
+      <c r="K110" s="15">
+        <v>1.4559</v>
+      </c>
+      <c r="L110" s="15">
+        <v>1.5405</v>
+      </c>
+      <c r="M110" s="15">
+        <v>1.6569</v>
+      </c>
       <c r="O110" s="1">
         <v>784</v>
       </c>
@@ -9552,7 +11307,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="111" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="1">
+        <v>24</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.2412</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0.44269999999999998</v>
+      </c>
+      <c r="E111" s="2">
+        <v>0.62390000000000001</v>
+      </c>
+      <c r="F111" s="2">
+        <v>0.83409999999999995</v>
+      </c>
+      <c r="G111" s="2">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="H111" s="2">
+        <v>1.0523</v>
+      </c>
+      <c r="I111" s="2">
+        <v>1.157</v>
+      </c>
+      <c r="J111" s="2">
+        <v>1.2523</v>
+      </c>
+      <c r="K111" s="2">
+        <v>1.3882000000000001</v>
+      </c>
+      <c r="L111" s="2">
+        <v>1.4847999999999999</v>
+      </c>
+      <c r="M111" s="2">
+        <v>1.6039000000000001</v>
+      </c>
       <c r="O111" s="1">
         <v>785</v>
       </c>
@@ -9597,7 +11388,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="112" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="1">
+        <v>25</v>
+      </c>
+      <c r="C112" s="15">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="D112" s="15">
+        <v>0.42970000000000003</v>
+      </c>
+      <c r="E112" s="15">
+        <v>0.64870000000000005</v>
+      </c>
+      <c r="F112" s="15">
+        <v>0.81020000000000003</v>
+      </c>
+      <c r="G112" s="15">
+        <v>0.9657</v>
+      </c>
+      <c r="H112" s="15">
+        <v>1.0465</v>
+      </c>
+      <c r="I112" s="15">
+        <v>1.1623000000000001</v>
+      </c>
+      <c r="J112" s="15">
+        <v>1.2602</v>
+      </c>
+      <c r="K112" s="15">
+        <v>1.3782000000000001</v>
+      </c>
+      <c r="L112" s="15">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="M112" s="15">
+        <v>1.5942000000000001</v>
+      </c>
       <c r="O112" s="1">
         <v>786</v>
       </c>
@@ -9642,7 +11469,43 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="113" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="1">
+        <v>26</v>
+      </c>
+      <c r="C113" s="2">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0.36149999999999999</v>
+      </c>
+      <c r="E113" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="F113" s="2">
+        <v>0.81659999999999999</v>
+      </c>
+      <c r="G113" s="2">
+        <v>0.96350000000000002</v>
+      </c>
+      <c r="H113" s="2">
+        <v>1.0592999999999999</v>
+      </c>
+      <c r="I113" s="2">
+        <v>1.1645000000000001</v>
+      </c>
+      <c r="J113" s="2">
+        <v>1.2419</v>
+      </c>
+      <c r="K113" s="2">
+        <v>1.3512</v>
+      </c>
+      <c r="L113" s="2">
+        <v>1.4528000000000001</v>
+      </c>
+      <c r="M113" s="2">
+        <v>1.5770999999999999</v>
+      </c>
       <c r="O113" s="1">
         <v>787</v>
       </c>
@@ -9687,7 +11550,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="114" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O114" s="1">
         <v>788</v>
       </c>
@@ -9732,7 +11595,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="115" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O115" s="1">
         <v>789</v>
       </c>
@@ -9777,7 +11640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O116" s="1">
         <v>790</v>
       </c>
@@ -9822,7 +11685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O117" s="1">
         <v>791</v>
       </c>
@@ -9867,7 +11730,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="118" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O118" s="1">
         <v>792</v>
       </c>
@@ -9912,7 +11775,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="119" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O119" s="1">
         <v>793</v>
       </c>
@@ -9957,7 +11820,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="120" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O120" s="1">
         <v>794</v>
       </c>
@@ -10002,7 +11865,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="121" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O121" s="1">
         <v>795</v>
       </c>
@@ -10047,7 +11910,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="122" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O122" s="1">
         <v>796</v>
       </c>
@@ -10092,7 +11955,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="123" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O123" s="1">
         <v>797</v>
       </c>
@@ -10137,7 +12000,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="124" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O124" s="1">
         <v>798</v>
       </c>
@@ -10182,7 +12045,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="125" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O125" s="1">
         <v>799</v>
       </c>
@@ -10227,7 +12090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O126" s="1">
         <v>800</v>
       </c>
@@ -10272,7 +12135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O127" s="1">
         <v>801</v>
       </c>
@@ -10317,7 +12180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="15:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O128" s="1">
         <v>802</v>
       </c>
@@ -15987,8 +17850,584 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
+    <row r="260" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O260" s="1">
+        <v>1255</v>
+      </c>
+      <c r="P260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Q260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="R260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="S260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="T260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="U260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="V260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="W260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="X260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Y260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Z260" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="AA260" s="15">
+        <v>0.18181818</v>
+      </c>
+      <c r="AB260" s="15">
+        <v>0.18181818</v>
+      </c>
+      <c r="AC260" s="13">
+        <f>SUM(P260:AB260)</f>
+        <v>0.400450786</v>
+      </c>
+    </row>
+    <row r="261" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O261" s="1">
+        <v>1256</v>
+      </c>
+      <c r="P261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Q261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="R261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="S261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="T261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="U261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="V261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="W261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="X261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Y261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Z261" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="AA261" s="2">
+        <v>0.18181818</v>
+      </c>
+      <c r="AB261" s="2">
+        <v>0.18181818</v>
+      </c>
+      <c r="AC261" s="13">
+        <f t="shared" ref="AC261:AC263" si="4">SUM(P261:AB261)</f>
+        <v>0.400450786</v>
+      </c>
+    </row>
+    <row r="262" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O262" s="1">
+        <v>1257</v>
+      </c>
+      <c r="P262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Q262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="R262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="S262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="T262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="U262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="V262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="W262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="X262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Y262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Z262" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="AA262" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB262" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC262" s="13">
+        <f t="shared" si="4"/>
+        <v>9.0909092999999996E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O263" s="1">
+        <v>1258</v>
+      </c>
+      <c r="P263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Q263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="R263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="S263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="T263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="U263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="V263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="W263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="X263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Y263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Z263" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="AA263" s="2">
+        <v>9.0909089999999998E-2</v>
+      </c>
+      <c r="AB263" s="2">
+        <v>9.0909089999999998E-2</v>
+      </c>
+      <c r="AC263" s="13">
+        <f t="shared" si="4"/>
+        <v>0.242674679</v>
+      </c>
+    </row>
+    <row r="265" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O265" s="1">
+        <v>1255</v>
+      </c>
+      <c r="P265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Q265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="R265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="S265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="T265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="U265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="V265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="W265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="X265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Y265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Z265" s="15">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="AC265" s="13">
+        <f>SUM(P265:AB265)</f>
+        <v>0.63636363999999979</v>
+      </c>
+    </row>
+    <row r="266" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O266" s="1">
+        <v>1256</v>
+      </c>
+      <c r="P266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Q266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="R266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="S266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="T266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="U266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="V266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="W266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="X266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Y266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="Z266" s="2">
+        <v>5.7851239999999998E-2</v>
+      </c>
+      <c r="AC266" s="13">
+        <f>SUM(P266:AB266)</f>
+        <v>0.63636363999999979</v>
+      </c>
+    </row>
+    <row r="267" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O267" s="1">
+        <v>1257</v>
+      </c>
+      <c r="P267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="Q267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="R267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="S267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="T267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="U267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="V267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="W267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="X267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="Y267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="Z267" s="15">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="AC267" s="13">
+        <f>SUM(P267:AB267)</f>
+        <v>1.0000000010000001</v>
+      </c>
+    </row>
+    <row r="268" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O268" s="1">
+        <v>1258</v>
+      </c>
+      <c r="P268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="Q268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="R268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="S268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="T268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="U268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="V268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="W268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="X268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="Y268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="Z268" s="2">
+        <v>7.4380164999999998E-2</v>
+      </c>
+      <c r="AC268" s="13">
+        <f>SUM(P268:AB268)</f>
+        <v>0.81818181499999998</v>
+      </c>
+    </row>
+    <row r="270" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O270" s="1">
+        <v>1255</v>
+      </c>
+      <c r="P270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Q270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="R270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="S270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="T270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="U270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="V270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="W270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="X270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Y270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Z270" s="14">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="AA270" s="15">
+        <v>0.31818182</v>
+      </c>
+      <c r="AB270" s="15">
+        <v>0.31818182</v>
+      </c>
+      <c r="AC270" s="13">
+        <f>SUM(P270:AB270)</f>
+        <v>0.67317806599999996</v>
+      </c>
+    </row>
+    <row r="271" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O271" s="1">
+        <v>1256</v>
+      </c>
+      <c r="P271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Q271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="R271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="S271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="T271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="U271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="V271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="W271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="X271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Y271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="Z271" s="16">
+        <v>3.3467660000000002E-3</v>
+      </c>
+      <c r="AA271" s="2">
+        <v>0.31818182</v>
+      </c>
+      <c r="AB271" s="2">
+        <v>0.31818182</v>
+      </c>
+      <c r="AC271" s="13">
+        <f>SUM(P271:AB271)</f>
+        <v>0.67317806599999996</v>
+      </c>
+    </row>
+    <row r="272" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O272" s="1">
+        <v>1257</v>
+      </c>
+      <c r="P272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Q272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="R272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="S272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="T272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="U272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="V272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="W272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="X272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Y272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="Z272" s="14">
+        <v>8.2644629999999997E-3</v>
+      </c>
+      <c r="AA272" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="AB272" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="AC272" s="13">
+        <f>SUM(P272:AB272)</f>
+        <v>1.0909090930000001</v>
+      </c>
+    </row>
+    <row r="273" spans="15:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O273" s="1">
+        <v>1258</v>
+      </c>
+      <c r="P273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Q273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="R273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="S273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="T273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="U273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="V273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="W273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="X273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Y273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="Z273" s="16">
+        <v>5.5324090000000003E-3</v>
+      </c>
+      <c r="AA273" s="2">
+        <v>0.40909090999999997</v>
+      </c>
+      <c r="AB273" s="2">
+        <v>0.40909090999999997</v>
+      </c>
+      <c r="AC273" s="13">
+        <f>SUM(P273:AB273)</f>
+        <v>0.87903831899999996</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L27">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:L56">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:L85">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -16000,7 +18439,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:L56">
+  <conditionalFormatting sqref="C88:M113">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>